<commit_message>
redmine #9195 Cal sheets updated/added for GP03FLMB deployments 1-3.
</commit_message>
<xml_diff>
--- a/GP03FLMB/Omaha_Cal_Info_GP03FLMB_00002.xlsx
+++ b/GP03FLMB/Omaha_Cal_Info_GP03FLMB_00002.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="2300" yWindow="1940" windowWidth="24960" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,12 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -171,18 +176,12 @@
     <t>GP03FLMB-00002</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>50° 19.88' N</t>
   </si>
   <si>
     <t>144° 23.85' W</t>
   </si>
   <si>
-    <t>MV1404</t>
-  </si>
-  <si>
     <t>??</t>
   </si>
   <si>
@@ -267,16 +266,62 @@
     <t>GP03FLMA-00001</t>
   </si>
   <si>
-    <t>GP03FLMB-FMM01-01-SIOENG000</t>
-  </si>
-  <si>
-    <t>GP03FLMB-FMS01-01-SIOENG000</t>
-  </si>
-  <si>
     <t>GP03FLMB-00002-FMS01</t>
   </si>
   <si>
     <t>GP03FLMB-00002-FMM01</t>
+  </si>
+  <si>
+    <t>MV-1404</t>
+  </si>
+  <si>
+    <r>
+      <t>GP03FLMB-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>M01-01-SIOENG000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GP03FLMB-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>S01-01-SIOENG000</t>
+    </r>
+  </si>
+  <si>
+    <t>Units in mm</t>
   </si>
 </sst>
 </file>
@@ -284,13 +329,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +538,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -574,16 +646,16 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,19 +674,19 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="132">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -678,14 +750,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -747,8 +819,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -783,22 +857,22 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -834,13 +908,13 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="28" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -895,8 +969,20 @@
     <xf numFmtId="0" fontId="31" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="132">
+  <cellStyles count="134">
     <cellStyle name="Comma 2" xfId="63"/>
     <cellStyle name="Comma 2 2" xfId="64"/>
     <cellStyle name="Comma 2 2 2" xfId="65"/>
@@ -907,6 +993,8 @@
     <cellStyle name="Currency 2 3" xfId="70"/>
     <cellStyle name="Excel Built-in Normal" xfId="6"/>
     <cellStyle name="Excel Built-in Normal 2" xfId="71"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="9"/>
     <cellStyle name="Hyperlink 2 2" xfId="72"/>
     <cellStyle name="Hyperlink 2 3" xfId="73"/>
@@ -1044,7 +1132,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1349,29 +1437,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="6"/>
+    <col min="7" max="7" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.5" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="28">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1406,19 +1494,19 @@
         <v>37</v>
       </c>
       <c r="L1" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="O1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" s="18" customFormat="1">
       <c r="A2" s="45" t="s">
         <v>47</v>
       </c>
@@ -1434,20 +1522,20 @@
       <c r="E2" s="31">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="51">
+        <v>42162</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="I2" s="5">
         <v>4145</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>52</v>
+      <c r="J2" s="50" t="s">
+        <v>81</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="32">
@@ -1459,23 +1547,28 @@
         <v>-144.39750000000001</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="18" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="18" customFormat="1">
       <c r="D3" s="28"/>
       <c r="E3" s="29"/>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:15" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" customFormat="1">
       <c r="A4" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1483,27 +1576,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="510" topLeftCell="A67" activePane="bottomLeft"/>
-      <selection activeCell="E1" sqref="E1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="11" customWidth="1"/>
-    <col min="8" max="11" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="11" customWidth="1"/>
+    <col min="8" max="11" width="10.6640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="2"/>
+    <col min="13" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="14" customFormat="1">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1626,7 @@
       <c r="L1" s="25"/>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
@@ -1547,9 +1641,9 @@
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>48</v>
@@ -1574,9 +1668,9 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>48</v>
@@ -1598,9 +1692,9 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>48</v>
@@ -1619,9 +1713,9 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>48</v>
@@ -1640,9 +1734,9 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>48</v>
@@ -1661,9 +1755,9 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>48</v>
@@ -1682,9 +1776,9 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>48</v>
@@ -1702,13 +1796,13 @@
         <v>124</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>48</v>
@@ -1726,13 +1820,13 @@
         <v>700</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="35" t="s">
         <v>48</v>
@@ -1750,13 +1844,13 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="35" t="s">
         <v>48</v>
@@ -1774,13 +1868,13 @@
         <v>3.9E-2</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>48</v>
@@ -1789,7 +1883,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>18</v>
@@ -1805,9 +1899,9 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>48</v>
@@ -1816,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>19</v>
@@ -1826,9 +1920,9 @@
       </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" s="35" t="s">
         <v>48</v>
@@ -1837,7 +1931,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>20</v>
@@ -1847,9 +1941,9 @@
       </c>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>48</v>
@@ -1858,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>21</v>
@@ -1868,9 +1962,9 @@
       </c>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="35" t="s">
         <v>48</v>
@@ -1879,7 +1973,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>22</v>
@@ -1889,9 +1983,9 @@
       </c>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>48</v>
@@ -1900,7 +1994,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>23</v>
@@ -1910,9 +2004,9 @@
       </c>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="35" t="s">
         <v>48</v>
@@ -1921,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>38</v>
@@ -1930,11 +2024,11 @@
         <v>35</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" s="37" t="s">
         <v>45</v>
       </c>
@@ -1961,7 +2055,7 @@
       </c>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="36" t="s">
         <v>45</v>
       </c>
@@ -1985,7 +2079,7 @@
       </c>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="36" t="s">
         <v>45</v>
       </c>
@@ -2002,13 +2096,13 @@
         <v>15</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>48</v>
@@ -2033,9 +2127,9 @@
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" s="35" t="s">
         <v>48</v>
@@ -2054,9 +2148,9 @@
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B25" s="35" t="s">
         <v>48</v>
@@ -2075,9 +2169,9 @@
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>48</v>
@@ -2096,9 +2190,9 @@
       </c>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>48</v>
@@ -2112,14 +2206,17 @@
       <c r="E27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="4">
-        <v>5010</v>
+      <c r="F27" s="52">
+        <v>500000</v>
+      </c>
+      <c r="G27" s="53" t="s">
+        <v>84</v>
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B28" s="35" t="s">
         <v>48</v>
@@ -2138,9 +2235,9 @@
       </c>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>48</v>
@@ -2159,9 +2256,9 @@
       </c>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>48</v>
@@ -2180,9 +2277,9 @@
       </c>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>48</v>
@@ -2201,9 +2298,9 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>48</v>
@@ -2227,9 +2324,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33" s="35" t="s">
         <v>48</v>
@@ -2247,9 +2344,9 @@
         <v>50.331333333333333</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" s="35" t="s">
         <v>48</v>
@@ -2267,9 +2364,9 @@
         <v>-144.39750000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="35" t="s">
         <v>48</v>
@@ -2281,15 +2378,15 @@
         <v>11646</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F35" s="4">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>48</v>
@@ -2313,9 +2410,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" s="35" t="s">
         <v>48</v>
@@ -2333,9 +2430,9 @@
         <v>50.331333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B38" s="35" t="s">
         <v>48</v>
@@ -2353,9 +2450,9 @@
         <v>-144.39750000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B39" s="35" t="s">
         <v>48</v>
@@ -2367,15 +2464,15 @@
         <v>11654</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F39" s="4">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>48</v>
@@ -2399,9 +2496,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B41" s="35" t="s">
         <v>48</v>
@@ -2419,9 +2516,9 @@
         <v>50.331333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B42" s="35" t="s">
         <v>48</v>
@@ -2439,9 +2536,9 @@
         <v>-144.39750000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B43" s="35" t="s">
         <v>48</v>
@@ -2453,15 +2550,15 @@
         <v>11653</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F43" s="4">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>48</v>
@@ -2486,9 +2583,9 @@
       </c>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" s="35" t="s">
         <v>48</v>
@@ -2507,9 +2604,9 @@
       </c>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" s="35" t="s">
         <v>48</v>
@@ -2528,9 +2625,9 @@
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B47" s="35" t="s">
         <v>48</v>
@@ -2542,16 +2639,16 @@
         <v>11641</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F47" s="4">
         <v>41</v>
       </c>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>48</v>
@@ -2576,9 +2673,9 @@
       </c>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B49" s="35" t="s">
         <v>48</v>
@@ -2597,9 +2694,9 @@
       </c>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B50" s="35" t="s">
         <v>48</v>
@@ -2618,9 +2715,9 @@
       </c>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B51" s="35" t="s">
         <v>48</v>
@@ -2632,16 +2729,16 @@
         <v>11650</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F51" s="4">
         <v>50</v>
       </c>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" s="37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>48</v>
@@ -2666,9 +2763,9 @@
       </c>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B53" s="35" t="s">
         <v>48</v>
@@ -2687,9 +2784,9 @@
       </c>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B54" s="35" t="s">
         <v>48</v>
@@ -2708,9 +2805,9 @@
       </c>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B55" s="35" t="s">
         <v>48</v>
@@ -2722,7 +2819,7 @@
         <v>11638</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F55" s="4">
         <v>38</v>
@@ -2731,9 +2828,9 @@
       <c r="K55" s="43"/>
       <c r="L55" s="43"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>48</v>
@@ -2760,9 +2857,9 @@
       <c r="K56" s="43"/>
       <c r="L56" s="43"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B57" s="35" t="s">
         <v>48</v>
@@ -2783,9 +2880,9 @@
       <c r="K57" s="43"/>
       <c r="L57" s="43"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B58" s="35" t="s">
         <v>48</v>
@@ -2806,9 +2903,9 @@
       <c r="K58" s="43"/>
       <c r="L58" s="43"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B59" s="35" t="s">
         <v>48</v>
@@ -2820,7 +2917,7 @@
         <v>11640</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F59" s="4">
         <v>40</v>
@@ -2829,9 +2926,9 @@
       <c r="K59" s="43"/>
       <c r="L59" s="43"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>48</v>
@@ -2858,9 +2955,9 @@
       <c r="K60" s="43"/>
       <c r="L60" s="43"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B61" s="35" t="s">
         <v>48</v>
@@ -2881,9 +2978,9 @@
       <c r="K61" s="43"/>
       <c r="L61" s="43"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B62" s="35" t="s">
         <v>48</v>
@@ -2904,9 +3001,9 @@
       <c r="K62" s="43"/>
       <c r="L62" s="43"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B63" s="35" t="s">
         <v>48</v>
@@ -2918,7 +3015,7 @@
         <v>11639</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F63" s="4">
         <v>39</v>
@@ -2927,9 +3024,9 @@
       <c r="K63" s="43"/>
       <c r="L63" s="43"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>48</v>
@@ -2956,9 +3053,9 @@
       <c r="K64" s="43"/>
       <c r="L64" s="43"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B65" s="35" t="s">
         <v>48</v>
@@ -2979,9 +3076,9 @@
       <c r="K65" s="43"/>
       <c r="L65" s="43"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B66" s="35" t="s">
         <v>48</v>
@@ -3002,9 +3099,9 @@
       <c r="K66" s="43"/>
       <c r="L66" s="43"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B67" s="35" t="s">
         <v>48</v>
@@ -3016,16 +3113,16 @@
         <v>10223</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F67" s="4">
         <v>23</v>
       </c>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" s="1" customFormat="1">
       <c r="A68" s="42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>48</v>
@@ -3050,9 +3147,9 @@
       </c>
       <c r="J68" s="40"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B69" s="38" t="s">
         <v>48</v>
@@ -3071,9 +3168,9 @@
       </c>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B70" s="38" t="s">
         <v>48</v>
@@ -3092,9 +3189,9 @@
       </c>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B71" s="38" t="s">
         <v>48</v>
@@ -3106,16 +3203,16 @@
         <v>10228</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F71" s="4">
         <v>28</v>
       </c>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>48</v>
@@ -3140,9 +3237,9 @@
       </c>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B73" s="35" t="s">
         <v>48</v>
@@ -3161,9 +3258,9 @@
       </c>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B74" s="35" t="s">
         <v>48</v>
@@ -3182,9 +3279,9 @@
       </c>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B75" s="35" t="s">
         <v>48</v>
@@ -3196,16 +3293,16 @@
         <v>11680</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F75" s="4">
         <v>80</v>
       </c>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>48</v>
@@ -3230,9 +3327,9 @@
       </c>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12">
       <c r="A77" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77" s="35" t="s">
         <v>48</v>
@@ -3251,9 +3348,9 @@
       </c>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12">
       <c r="A78" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B78" s="35" t="s">
         <v>48</v>
@@ -3272,9 +3369,9 @@
       </c>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B79" s="35" t="s">
         <v>48</v>
@@ -3286,40 +3383,40 @@
         <v>11703</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F79" s="4">
         <v>3</v>
       </c>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12">
       <c r="A80" s="46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B80" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="48">
+        <v>2</v>
+      </c>
+      <c r="D80" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C80" s="48">
-        <v>2</v>
-      </c>
-      <c r="D80" s="49" t="s">
-        <v>84</v>
-      </c>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81" s="46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B81" s="47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C81" s="48">
         <v>2</v>
       </c>
       <c r="D81" s="49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E81" s="26"/>
       <c r="F81" s="26"/>
@@ -3331,7 +3428,7 @@
       <c r="L81" s="26"/>
       <c r="M81" s="26"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13">
       <c r="A82" s="26"/>
       <c r="B82" s="26"/>
       <c r="C82" s="27"/>
@@ -3346,7 +3443,7 @@
       <c r="L82" s="26"/>
       <c r="M82" s="26"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13">
       <c r="A83" s="26"/>
       <c r="B83" s="26"/>
       <c r="C83" s="27"/>
@@ -3361,7 +3458,7 @@
       <c r="L83" s="26"/>
       <c r="M83" s="26"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13">
       <c r="A84" s="26"/>
       <c r="B84" s="26"/>
       <c r="C84" s="27"/>
@@ -3378,6 +3475,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>